<commit_message>
login failed error massage genrate
</commit_message>
<xml_diff>
--- a/src/assets/sampleExcel/Bulk Upload Sample.xlsx
+++ b/src/assets/sampleExcel/Bulk Upload Sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rabiussanym\OneDrive - MetLife\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rabiussanym\OneDrive - MetLife\Documents\ULM_repo_1\13639-ULM-client\src\assets\sampleExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C079EB8-AD21-4C8C-8682-2BA1992E365A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACC7129-9829-47D6-9B4F-213DD897CF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>Customer Firstname</t>
   </si>
@@ -284,36 +284,6 @@
   </si>
   <si>
     <t>Tax Calculator</t>
-  </si>
-  <si>
-    <t>Sakib</t>
-  </si>
-  <si>
-    <t>Al Hasan</t>
-  </si>
-  <si>
-    <t>sakibalhasan@gmail.cokm</t>
-  </si>
-  <si>
-    <t>8801405628221</t>
-  </si>
-  <si>
-    <t>Mushfiq</t>
-  </si>
-  <si>
-    <t>Rahim</t>
-  </si>
-  <si>
-    <t>8801405628222</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tahim </t>
-  </si>
-  <si>
-    <t>Iqbal</t>
-  </si>
-  <si>
-    <t>8801405628223</t>
   </si>
 </sst>
 </file>
@@ -686,7 +656,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -745,60 +715,13 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C5" s="2"/>
@@ -813,11 +736,8 @@
       <c r="C10" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{D2DAEAEC-FA82-421A-B1C7-D795628D45DF}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -1432,20 +1352,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="838852be-5671-4671-91c1-e2a96c5b6e3d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="838852be-5671-4671-91c1-e2a96c5b6e3d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1468,14 +1388,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F9E68D5-718A-494D-BCC4-BA1EC8EABBBC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87AF3F94-942A-4541-80E7-96CAA59C38DE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -1490,4 +1402,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F9E68D5-718A-494D-BCC4-BA1EC8EABBBC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>